<commit_message>
update converter and dictionary
</commit_message>
<xml_diff>
--- a/manchu-korean.xlsx
+++ b/manchu-korean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vv137/Repos/manchu-dict/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCDCA3F-E5B7-4847-9EE6-C7E9C0C49448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88E6996-C856-474C-8778-A26B44EBB3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32000" yWindow="500" windowWidth="32000" windowHeight="35500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="137">
   <si>
     <t>id</t>
   </si>
@@ -38,10 +38,400 @@
     <t>meaning_ko</t>
   </si>
   <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A FA SERE ONGGOLO</t>
+  </si>
+  <si>
+    <t>a si</t>
+  </si>
+  <si>
+    <t>A SI</t>
+  </si>
+  <si>
+    <t>a ta</t>
+  </si>
+  <si>
+    <t>A TA</t>
+  </si>
+  <si>
+    <t>aba</t>
+  </si>
+  <si>
+    <t>ABA</t>
+  </si>
+  <si>
+    <t>abalabumbi</t>
+  </si>
+  <si>
+    <t>ABALABUMBI</t>
+  </si>
+  <si>
+    <t>abalambi</t>
+  </si>
+  <si>
+    <t>ABALAMBI</t>
+  </si>
+  <si>
+    <t>abalanambi</t>
+  </si>
+  <si>
+    <t>ABALANAMBI</t>
+  </si>
+  <si>
+    <t>abalanjimbi</t>
+  </si>
+  <si>
+    <t>ABALANJIMBI</t>
+  </si>
+  <si>
+    <t>abdaha</t>
+  </si>
+  <si>
+    <t>ABDAHA</t>
+  </si>
+  <si>
+    <t>abdahanambi</t>
+  </si>
+  <si>
+    <t>ABDAHANAMBI</t>
+  </si>
+  <si>
+    <t>abdangga</t>
+  </si>
+  <si>
+    <t>ABDANGGA</t>
+  </si>
+  <si>
+    <t>abdari</t>
+  </si>
+  <si>
+    <t>ABDARI</t>
+  </si>
+  <si>
+    <t>abgari</t>
+  </si>
+  <si>
+    <t>ABGARI</t>
+  </si>
+  <si>
     <t>manchu</t>
   </si>
   <si>
     <t>translation_ko</t>
+  </si>
+  <si>
+    <t>A -I BUKDAN</t>
+  </si>
+  <si>
+    <t>A JIJUN -I ACANGGA</t>
+  </si>
+  <si>
+    <t>A JILGAN</t>
+  </si>
+  <si>
+    <t>ABA BARGIYAMBI</t>
+  </si>
+  <si>
+    <t>ABA SAHA</t>
+  </si>
+  <si>
+    <t>ABA SARAMBI</t>
+  </si>
+  <si>
+    <t>ABA SINDAMBI</t>
+  </si>
+  <si>
+    <t>ABA TUCIMBI</t>
+  </si>
+  <si>
+    <t>자아(字牙). 만주 문자에서 한쪽으로 튀어나온 획.</t>
+  </si>
+  <si>
+    <t>A E</t>
+  </si>
+  <si>
+    <t>양(陽)과 음(陰).</t>
+  </si>
+  <si>
+    <t>A -I JALAN</t>
+  </si>
+  <si>
+    <t>접은 종이의 바깥 면, 접은 종이의 표면. 양구(陽扣).</t>
+  </si>
+  <si>
+    <t>이 세상, 현세. 陽世.</t>
+  </si>
+  <si>
+    <t>A -I TON</t>
+  </si>
+  <si>
+    <t>양수. 陽數.</t>
+  </si>
+  <si>
+    <t>양(陽). 음양(陰陽)의 양(陽).</t>
+  </si>
+  <si>
+    <t>A JIJUN</t>
+  </si>
+  <si>
+    <t>양각 글자. 陽文.</t>
+  </si>
+  <si>
+    <t>양각 글자의 합부(合符). 陽文合符. 구리로 만들어 內府에 보관하며 밤에 城門을 통행하기 위해 휴대함.</t>
+  </si>
+  <si>
+    <t>[음악] 양성(陽聲). 十二律가운데서 六律의 소리.</t>
+  </si>
+  <si>
+    <t>아. 어. 놀라거나 대답할 때 내는 소리.</t>
+  </si>
+  <si>
+    <t>亞의 음사.</t>
+  </si>
+  <si>
+    <t>A U</t>
+  </si>
+  <si>
+    <t>[LA] AVE. AVE MARIA(亞物瑪利亞)의 AVE.</t>
+  </si>
+  <si>
+    <t>A SI SEME</t>
+  </si>
+  <si>
+    <t>구구. (닭을 쫓거나 부를 때 내는 소리.)</t>
+  </si>
+  <si>
+    <t>왁자지껄. (시끄러운 분위기를 내는 소리.)</t>
+  </si>
+  <si>
+    <t>구구 하며. / 왁자지껄하게.</t>
+  </si>
+  <si>
+    <t>A TA SEME</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>예예, 그래그래. 놀라거나 대답할 때 내는 소리.</t>
+  </si>
+  <si>
+    <t>ABA ABALAMBI</t>
+  </si>
+  <si>
+    <t>몰이사냥, 포위 수렵. 圍獵.</t>
+  </si>
+  <si>
+    <t>몰이사냥하다, 몰이사냥의 포위 대열을 배치하다. 打圍.</t>
+  </si>
+  <si>
+    <t>몰이사냥을 끝내다, 몰이사냥의 포위 대열을 거두어들이다. 收圍.</t>
+  </si>
+  <si>
+    <t>ABA DE TUCIBUMBI</t>
+  </si>
+  <si>
+    <t>몰이사냥에 보내다.</t>
+  </si>
+  <si>
+    <t>ABA HOIHAN</t>
+  </si>
+  <si>
+    <t>수렵장, 사냥터. 圍場.</t>
+  </si>
+  <si>
+    <t>ABA -I BA</t>
+  </si>
+  <si>
+    <t>몰이사냥. =`aba`.</t>
+  </si>
+  <si>
+    <t>A'니 'FA'니 하기 전에, 누구보다 먼저, 가장 먼저. =`afanggala`.</t>
+  </si>
+  <si>
+    <t>어디, 어느 곳, 어디 있는가. =`aiba`.</t>
+  </si>
+  <si>
+    <t>포위 대열을 펼치다, 사냥의 포위 대열을 두 방향으로 벌려 가다. 撒圍.</t>
+  </si>
+  <si>
+    <t>포위 대열을 치다, 몰이사냥의 포위 대열의 중앙부에서 양끝으로 한 사람씩 나와서 兩翼을 만들어 가다. 放圍.</t>
+  </si>
+  <si>
+    <t>몰이사냥을 가다.</t>
+  </si>
+  <si>
+    <t>ABA NIYALMA</t>
+  </si>
+  <si>
+    <t>몰이사냥을 하는 사람.</t>
+  </si>
+  <si>
+    <t>BEILE ABA</t>
+  </si>
+  <si>
+    <t>Beile는 어디 있는가?</t>
+  </si>
+  <si>
+    <t>abaga</t>
+  </si>
+  <si>
+    <t>ABAGA</t>
+  </si>
+  <si>
+    <t>abaganar</t>
+  </si>
+  <si>
+    <t>ABAGANAR</t>
+  </si>
+  <si>
+    <t>阿巴噶. 내몽고의 部의 하나. 청대 2旗로 편제됨. Abaqa ayimaγ. 몽골어로 '부계 혈통을 잇는 사람'이라는 뜻에서 유래함. 칭기스칸의 동생 벨구테이(別里古台, Belgutei)의 후손임.</t>
+  </si>
+  <si>
+    <t>阿巴哈納爾. 내몽고의 部의 하나. 청대 2旗로 편제됨. Abaqanar ayimaγ. 만주어로 Abahanar라고도 함. 칭기스칸의 동생 벨구테이(別里古台, Belgutei)의 후손임.</t>
+  </si>
+  <si>
+    <t>abai</t>
+  </si>
+  <si>
+    <t>ABAI</t>
+  </si>
+  <si>
+    <t>(몽) 여동생. 妹.</t>
+  </si>
+  <si>
+    <t>Abai</t>
+  </si>
+  <si>
+    <t>(인명) 鎮國勤敏公 阿拜. 청태조의 3남. 清史稿/卷217 참고.</t>
+  </si>
+  <si>
+    <t>abalahai</t>
+  </si>
+  <si>
+    <t>(`abalambi`의 사동형) 몰이사냥으 하게 하다.</t>
+  </si>
+  <si>
+    <t>ABALAHAI</t>
+  </si>
+  <si>
+    <t>(`abalambi`의 부사형) 몰이사냥하면서.</t>
+  </si>
+  <si>
+    <t>몰이사냥하다.</t>
+  </si>
+  <si>
+    <t>ABALAME GENEMBI</t>
+  </si>
+  <si>
+    <t>몰이사냥하러 가다.</t>
+  </si>
+  <si>
+    <t>ABALAME YABUMBI</t>
+  </si>
+  <si>
+    <t>KAME ABALAMBI</t>
+  </si>
+  <si>
+    <t>겨울 사냥을 하다. 冬狩.</t>
+  </si>
+  <si>
+    <t>SONJOME ABALAMBI</t>
+  </si>
+  <si>
+    <t>봄에 임신하지 않은 짐승을 골라서 사냥하다, 봄 사냥을 하다. 春蒐.</t>
+  </si>
+  <si>
+    <t>ULUN GIDAMBI</t>
+  </si>
+  <si>
+    <t>여름 사냥을 하다, 여름에 곡물을 황폐하게 만드는 짐승을 잡다. 夏苗.</t>
+  </si>
+  <si>
+    <t>WAME ABALAMBI</t>
+  </si>
+  <si>
+    <t>가을 사냥을 하다. 秋獮. =`sahadambi`.</t>
+  </si>
+  <si>
+    <t>몰이사냥하러 가다, 가서 물이사냥하다.</t>
+  </si>
+  <si>
+    <t>abalandumbi</t>
+  </si>
+  <si>
+    <t>ABALANDUMBI</t>
+  </si>
+  <si>
+    <t>일제히 몰이사냥하다. =`abalanumbi`.</t>
+  </si>
+  <si>
+    <t>몰이사냥하러 오다, 와서 몰이사냥하다.</t>
+  </si>
+  <si>
+    <t>abalanumbi</t>
+  </si>
+  <si>
+    <t>ABALANUMBI</t>
+  </si>
+  <si>
+    <t>일제히 몰이사냥하다. =`abalandumbi`.</t>
+  </si>
+  <si>
+    <t>Abatai</t>
+  </si>
+  <si>
+    <t>ABATAI</t>
+  </si>
+  <si>
+    <t>(인명) 饒餘敏郡王 阿巴泰. 청태조의 7남. 清史稿/卷217 참고.</t>
+  </si>
+  <si>
+    <t>잎. 葉.</t>
+  </si>
+  <si>
+    <t>싹트다, 싹이 나다.</t>
+  </si>
+  <si>
+    <t>abdalabumbi</t>
+  </si>
+  <si>
+    <t>ABDALABUMBI</t>
+  </si>
+  <si>
+    <t>(`abdalambi`의 사동형) 꺾어 취하게 하다.</t>
+  </si>
+  <si>
+    <t>책(冊). 책봉(冊封)하거나 조서(詔書)를 내릴 때 사용하며 접은 형태임.</t>
+  </si>
+  <si>
+    <t>잎이 큰.</t>
+  </si>
+  <si>
+    <t>abdarakv</t>
+  </si>
+  <si>
+    <t>ABDARAKV</t>
+  </si>
+  <si>
+    <t>(`abdambi`의 부정형) 꺾지 않다, 꺾지 않는.</t>
+  </si>
+  <si>
+    <t>(식물) 상수리나무. 婆蘿柯, 柞樹.</t>
+  </si>
+  <si>
+    <t>(지명) 阿布達里崗. `abdari ala`. 압록강의 북쪽에 위치함. 랴오닝성 환런 만족 자치현에 위치함.</t>
+  </si>
+  <si>
+    <t>한가한, 일이 없는. 임관(任官)하지 않고 한거(閑居)하는.</t>
   </si>
 </sst>
 </file>
@@ -77,8 +467,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -412,6 +803,550 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" t="s">
+        <v>132</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -419,9 +1354,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -435,10 +1372,318 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>